<commit_message>
fikser fordeling av restbeløp
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling-nyteknking.xlsx
+++ b/doc/okonomi/Utbetaling-nyteknking.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/dev/nav/helse-spleis/doc/okonomi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5294916-BB8A-1244-847B-C946FC9BA37C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015168BD-2C1C-D848-A1FB-3D0518520C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="500" windowWidth="32360" windowHeight="20360" xr2:uid="{D68530E5-53F4-9147-B78C-2EE89FEB1D81}"/>
+    <workbookView xWindow="15560" yWindow="7880" windowWidth="39420" windowHeight="21560" xr2:uid="{D68530E5-53F4-9147-B78C-2EE89FEB1D81}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
   <si>
     <t>Månedsinntekt</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>Alt over denne linjen er ting Vilkårsgrunnlag kan svare på</t>
-  </si>
-  <si>
-    <t>Beløp/verdier som ikke brukes</t>
   </si>
   <si>
     <t>Beløp som settes på Økonomi av Sykepengegrunnlag</t>
@@ -185,8 +182,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;NOK&quot;\ * #,##0.00_-;\-&quot;NOK&quot;\ * #,##0.00_-;_-&quot;NOK&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="0.0000%"/>
-    <numFmt numFmtId="172" formatCode="0.00000%"/>
+    <numFmt numFmtId="164" formatCode="0.0000%"/>
+    <numFmt numFmtId="165" formatCode="0.00000%"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -226,7 +223,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,12 +239,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -299,7 +290,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -311,26 +302,23 @@
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -649,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FF1C860-80D7-1E4E-BCDB-1C6933AA76C9}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -691,11 +679,9 @@
       <c r="E4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -706,16 +692,16 @@
         <v>26010.616666666669</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>8000</v>
       </c>
       <c r="E5" s="1">
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" s="4">
         <f>MIN(12*SUM(C5:E5),B2)</f>
-        <v>312127.40000000002</v>
+        <v>468127.4</v>
       </c>
       <c r="C6" s="4"/>
     </row>
@@ -725,15 +711,15 @@
       </c>
       <c r="C7" s="3">
         <f>C5/SUM($C$5:$E$5)</f>
-        <v>1</v>
+        <v>0.66675738271248386</v>
       </c>
       <c r="D7" s="3">
         <f>D5/SUM($C$5:$E$5)</f>
-        <v>0</v>
+        <v>0.20507237986924071</v>
       </c>
       <c r="E7" s="3">
         <f>E5/SUM($C$5:$E$5)</f>
-        <v>0</v>
+        <v>0.12817023741827543</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -747,14 +733,14 @@
       </c>
       <c r="D8" s="8">
         <f>$B$6*D7/12</f>
-        <v>0</v>
+        <v>8000</v>
       </c>
       <c r="E8" s="8">
         <f>$B$6*E7/12</f>
-        <v>0</v>
+        <v>4999.9999999999991</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -763,18 +749,18 @@
       </c>
       <c r="C9" s="3">
         <f>C8/SUM($C$8:$E$8)</f>
-        <v>1</v>
+        <v>0.66675738271248386</v>
       </c>
       <c r="D9" s="3">
         <f>D8/SUM($C$8:$E$8)</f>
-        <v>0</v>
+        <v>0.20507237986924071</v>
       </c>
       <c r="E9" s="3">
         <f>E8/SUM($C$8:$E$8)</f>
-        <v>0</v>
+        <v>0.12817023741827543</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -783,37 +769,35 @@
       </c>
       <c r="B10" s="8">
         <f>12*SUM(C8:E8)</f>
-        <v>312127.40000000002</v>
+        <v>468127.4</v>
       </c>
       <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="14">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="11">
         <f>C5</f>
         <v>26010.616666666669</v>
       </c>
-      <c r="D11" s="14">
-        <f t="shared" ref="D11:E11" si="0">D5</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="D11" s="11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="11">
+        <f t="shared" ref="D11:E11" si="0">E5</f>
+        <v>5000</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" s="4">
         <f>12*SUM(C11:E11)</f>
-        <v>312127.40000000002</v>
+        <v>372127.4</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="2">
         <v>1</v>
@@ -827,43 +811,43 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1">
         <f>MIN(C5*C13,C11)</f>
         <v>26010.616666666669</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" ref="D14:E14" si="1">MIN(D5*D13,D11)</f>
+        <f>MIN(D5*D13,D11)</f>
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ref="D14:E14" si="1">MIN(E5*E13,E11)</f>
+        <v>5000</v>
       </c>
       <c r="F14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="9"/>
-      <c r="C15" s="15">
+      <c r="C15" s="12">
         <f>IF(C5&gt;0,C14/C5,0)</f>
         <v>1</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="12">
         <f t="shared" ref="D15:E15" si="2">IF(D5&gt;0,D14/D5,0)</f>
         <v>0</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -872,7 +856,7 @@
       </c>
       <c r="C16" s="3">
         <f>C14/SUM($C$14:$E$14)</f>
-        <v>1</v>
+        <v>0.83876489610816085</v>
       </c>
       <c r="D16" s="3">
         <f t="shared" ref="D16:E16" si="3">D14/SUM($C$14:$E$14)</f>
@@ -880,92 +864,91 @@
       </c>
       <c r="E16" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.16123510389183918</v>
       </c>
       <c r="F16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="22" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="13" t="s">
+      <c r="A20" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="16">
+      <c r="C20" s="13">
         <f>(C8*C15)/SUMPRODUCT($C$8:$E$8,$C$15:$E$15)</f>
-        <v>1</v>
-      </c>
-      <c r="D20" s="16">
+        <v>0.83876489610816085</v>
+      </c>
+      <c r="D20" s="13">
         <f>(D8*D15)/SUMPRODUCT($C$8:$E$8,$C$15:$E$15)</f>
         <v>0</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E20" s="13">
         <f>(E8*E15)/SUMPRODUCT($C$8:$E$8,$C$15:$E$15)</f>
-        <v>0</v>
+        <v>0.16123510389183915</v>
       </c>
       <c r="F20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="13" t="s">
-        <v>34</v>
+      <c r="A21" t="s">
+        <v>33</v>
       </c>
       <c r="B21" s="4"/>
-      <c r="C21" s="17">
+      <c r="C21" s="14">
         <f>(1-C15)</f>
         <v>0</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21" s="14">
         <f>(1-D15)</f>
         <v>1</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E21" s="14">
         <f>(1-E15)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="13">
+        <f>IF(SUMPRODUCT($C$8:$E$8,$C$21:$E$21)&gt;0,(C8*C21)/SUMPRODUCT($C$8:$E$8,$C$21:$E$21),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="13">
+        <f t="shared" ref="D22:E22" si="4">IF(SUMPRODUCT($C$8:$E$8,$C$21:$E$21)&gt;0,(D8*D21)/SUMPRODUCT($C$8:$E$8,$C$21:$E$21),0)</f>
         <v>1</v>
       </c>
-      <c r="F21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="16">
-        <f>IF(SUMPRODUCT($C$8:$E$8,$C$21:$E$21)&gt;0,(C8*C21)/SUMPRODUCT($C$8:$E$8,$C$21:$E$21),0)</f>
-        <v>0</v>
-      </c>
-      <c r="D22" s="16">
-        <f t="shared" ref="D22:E22" si="4">IF(SUMPRODUCT($C$8:$E$8,$C$21:$E$21)&gt;0,(D8*D21)/SUMPRODUCT($C$8:$E$8,$C$21:$E$21),0)</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="16">
+      <c r="E22" s="13">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -978,7 +961,7 @@
         <v>0.5</v>
       </c>
       <c r="D24" s="2">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E24" s="2">
         <v>1</v>
@@ -991,45 +974,45 @@
       </c>
       <c r="C25" s="6">
         <f>C24*C9</f>
-        <v>0.5</v>
+        <v>0.33337869135624193</v>
       </c>
       <c r="D25" s="6">
         <f>D24*D9</f>
-        <v>0</v>
+        <v>0.16405790389539257</v>
       </c>
       <c r="E25" s="6">
         <f>E24*E9</f>
-        <v>0</v>
+        <v>0.12817023741827543</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" s="9"/>
-      <c r="C27" s="18">
+      <c r="C27" s="15">
         <f>(C20*C24) / SUMPRODUCT($C$20:$E$20,$C$24:$E$24)</f>
-        <v>1</v>
-      </c>
-      <c r="D27" s="18">
+        <v>0.72230411679518591</v>
+      </c>
+      <c r="D27" s="15">
         <f>(D20*D24) / SUMPRODUCT($C$20:$E$20,$C$24:$E$24)</f>
         <v>0</v>
       </c>
-      <c r="E27" s="18">
+      <c r="E27" s="15">
         <f>(E20*E24) / SUMPRODUCT($C$20:$E$20,$C$24:$E$24)</f>
-        <v>0</v>
+        <v>0.27769588320481409</v>
       </c>
       <c r="F27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28" s="3">
         <f>C11*C24/SUMPRODUCT($C11:$E$11,$C$24:$E$24)</f>
-        <v>1</v>
+        <v>0.72230411679518591</v>
       </c>
       <c r="D28" s="3">
         <f>D11*D24/SUMPRODUCT($C11:$E$11,$C$24:$E$24)</f>
@@ -1037,27 +1020,27 @@
       </c>
       <c r="E28" s="3">
         <f>E11*E24/SUMPRODUCT($C11:$E$11,$C$24:$E$24)</f>
-        <v>0</v>
+        <v>0.27769588320481414</v>
       </c>
       <c r="F28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29" s="9"/>
-      <c r="C29" s="15">
+      <c r="C29" s="12">
         <f>IF(SUMPRODUCT($C$22:$E$22,$C$24:$E$24)&gt;0,(C22*C24) / SUMPRODUCT($C$22:$E$22,$C$24:$E$24),0)</f>
         <v>0</v>
       </c>
-      <c r="D29" s="15">
-        <f t="shared" ref="D29:E29" si="5">IF(SUMPRODUCT($C$22:$E$22,$C$24:$E$24)&gt;0,(D22*D24) / SUMPRODUCT($C$22:$E$22,$C$24:$E$24),0)</f>
-        <v>0</v>
-      </c>
-      <c r="E29" s="15">
-        <f t="shared" si="5"/>
+      <c r="D29" s="12">
+        <f>IF(SUMPRODUCT($C$22:$E$22,$C$24:$E$24)&gt;0,(D22*D24) / SUMPRODUCT($C$22:$E$22,$C$24:$E$24),0)</f>
+        <v>1</v>
+      </c>
+      <c r="E29" s="12">
+        <f t="shared" ref="D29:E29" si="5">IF(SUMPRODUCT($C$22:$E$22,$C$24:$E$24)&gt;0,(E22*E24) / SUMPRODUCT($C$22:$E$22,$C$24:$E$24),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1069,9 +1052,9 @@
       <c r="A32" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="20">
+      <c r="B32" s="16">
         <f>SUM(C25:E25)</f>
-        <v>0.5</v>
+        <v>0.62560683266991002</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1082,13 +1065,13 @@
         <v>14</v>
       </c>
       <c r="B33" s="1">
-        <f>ROUND((12*SUMPRODUCT(C8:E8,C24:E24))/260,)*260</f>
-        <v>156000</v>
+        <f>ROUND((12*SUMPRODUCT(C14:E14,C24:E24))/260,)*260</f>
+        <v>216060</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="3"/>
       <c r="F33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1097,32 +1080,32 @@
       </c>
       <c r="B34" s="4">
         <f>ROUND(B10*B32/260,)*260</f>
-        <v>156000</v>
+        <v>292760</v>
       </c>
       <c r="C34" s="4">
         <f>B34/260</f>
-        <v>600</v>
+        <v>1126</v>
       </c>
       <c r="F34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B35" s="4">
         <f>MIN(B33,B34)</f>
-        <v>156000</v>
+        <v>216060</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B36" s="4">
         <f>B34-B35</f>
-        <v>0</v>
+        <v>76700</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -1130,304 +1113,303 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C37" s="4"/>
-      <c r="D37" s="21"/>
+      <c r="D37" s="17"/>
       <c r="E37" s="4"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B38" s="22"/>
-      <c r="C38" s="24">
+      <c r="A38" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="18"/>
+      <c r="C38" s="20">
         <f>$B$35*C27/260</f>
-        <v>600</v>
-      </c>
-      <c r="D38" s="24">
+        <v>600.23472105679957</v>
+      </c>
+      <c r="D38" s="20">
         <f>$B$35*D27/260</f>
         <v>0</v>
       </c>
-      <c r="E38" s="24">
+      <c r="E38" s="20">
         <f>$B$35*E27/260</f>
-        <v>0</v>
-      </c>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22">
+        <v>230.76527894320049</v>
+      </c>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18">
         <f>SUM(C38:E38)</f>
-        <v>600</v>
+        <v>831</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B39" s="22"/>
-      <c r="C39" s="24">
+      <c r="A39" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="18"/>
+      <c r="C39" s="20">
         <f>$B$36*C29/260</f>
         <v>0</v>
       </c>
-      <c r="D39" s="24">
+      <c r="D39" s="20">
         <f>$B$36*D29/260</f>
-        <v>0</v>
-      </c>
-      <c r="E39" s="24">
+        <v>295</v>
+      </c>
+      <c r="E39" s="20">
         <f>$B$36*E29/260</f>
         <v>0</v>
       </c>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22">
+      <c r="F39" s="18"/>
+      <c r="G39" s="18">
         <f>SUM(C39:E39)</f>
-        <v>0</v>
+        <v>295</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="22"/>
-      <c r="B40" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C40" s="24">
+      <c r="A40" s="18"/>
+      <c r="B40" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="20">
         <f>SUM(C38:C39)</f>
-        <v>600</v>
-      </c>
-      <c r="D40" s="24">
+        <v>600.23472105679957</v>
+      </c>
+      <c r="D40" s="20">
         <f t="shared" ref="D40:E40" si="6">SUM(D38:D39)</f>
-        <v>0</v>
-      </c>
-      <c r="E40" s="24">
+        <v>295</v>
+      </c>
+      <c r="E40" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22">
+        <v>230.76527894320049</v>
+      </c>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18">
         <f>SUM(G38:G39)</f>
-        <v>600</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="22"/>
-      <c r="B41" s="22"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="22"/>
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="22" t="s">
+      <c r="A42" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B42" s="22"/>
-      <c r="C42" s="24">
+      <c r="B42" s="18"/>
+      <c r="C42" s="20">
         <f>TRUNC(C38)</f>
         <v>600</v>
       </c>
-      <c r="D42" s="24">
+      <c r="D42" s="20">
         <f t="shared" ref="D42:E42" si="7">TRUNC(D38)</f>
         <v>0</v>
       </c>
-      <c r="E42" s="24">
+      <c r="E42" s="20">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="F42" s="22"/>
-      <c r="G42" s="22"/>
+        <v>230</v>
+      </c>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="22" t="s">
+      <c r="A43" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="18"/>
+      <c r="C43" s="20">
+        <f>C38-C42</f>
+        <v>0.23472105679957167</v>
+      </c>
+      <c r="D43" s="20">
+        <f t="shared" ref="D43:E43" si="8">D38-D42</f>
+        <v>0</v>
+      </c>
+      <c r="E43" s="20">
+        <f t="shared" si="8"/>
+        <v>0.76527894320048517</v>
+      </c>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B43" s="22"/>
-      <c r="C43" s="24">
-        <f>C38-C42</f>
-        <v>0</v>
-      </c>
-      <c r="D43" s="24">
-        <f t="shared" ref="D43:E43" si="8">D38-D42</f>
-        <v>0</v>
-      </c>
-      <c r="E43" s="24">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="F43" s="22"/>
-      <c r="G43" s="22"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="22" t="s">
+      <c r="B44" s="20">
+        <f>ROUND(SUM(C38:E38)-SUM(C42:E42),)</f>
+        <v>1</v>
+      </c>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="24">
-        <f>ROUND(SUM(C38:E38)-SUM(C42:E42),)</f>
-        <v>0</v>
-      </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="22"/>
-      <c r="G44" s="22"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="22" t="s">
+      <c r="B45" s="18"/>
+      <c r="C45" s="20">
+        <f>IF($B$44&gt;0,IF(LARGE($C$43:$F$43,$B$44)&lt;=C$43,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D45" s="20">
+        <f>IF(($B$44-C45)&gt;0,IF(LARGE($C$43:$F$43,$B$44)&lt;=D$43,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E45" s="20">
+        <f>IF(($B$44-SUM($C$45:$D$45))&gt;0,IF(LARGE($C$43:$F$43,$B$44)&lt;=E$43,1,0), 0)</f>
+        <v>1</v>
+      </c>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="22"/>
-      <c r="C45" s="24">
-        <f>IF($B$44&gt;0,IF(LARGE($C$43:$F$43,$B$44)&lt;=C$43,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D45" s="24">
-        <f>IF(($B$44-C43)&gt;0,IF(LARGE($C$42:$F$42,$B$44)&lt;=D$43,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E45" s="24">
-        <f>IF(($B$44-SUM($C$43:$D$43))&gt;0,IF(LARGE($C$42:$F$42,$B$44)&lt;=E$43,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F45" s="22"/>
-      <c r="G45" s="22"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="B46" s="23"/>
-      <c r="C46" s="23">
+      <c r="B46" s="19"/>
+      <c r="C46" s="19">
         <f>C42+C45</f>
         <v>600</v>
       </c>
-      <c r="D46" s="23">
+      <c r="D46" s="19">
         <f t="shared" ref="D46:E46" si="9">D42+D45</f>
         <v>0</v>
       </c>
-      <c r="E46" s="23">
+      <c r="E46" s="19">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="F46" s="23"/>
-      <c r="G46" s="23">
+        <v>231</v>
+      </c>
+      <c r="F46" s="19"/>
+      <c r="G46" s="19">
         <f>SUM(C46:E46)</f>
-        <v>600</v>
+        <v>831</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="22"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="22"/>
-      <c r="G47" s="22"/>
+      <c r="A47" s="18"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B48" s="24"/>
-      <c r="C48" s="24">
+      <c r="A48" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20">
         <f>TRUNC(C39)</f>
         <v>0</v>
       </c>
-      <c r="D48" s="24">
+      <c r="D48" s="20">
         <f t="shared" ref="D48:E48" si="10">TRUNC(D39)</f>
-        <v>0</v>
-      </c>
-      <c r="E48" s="24">
+        <v>295</v>
+      </c>
+      <c r="E48" s="20">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="F48" s="22"/>
-      <c r="G48" s="22"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="22" t="s">
+      <c r="A49" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B49" s="20"/>
+      <c r="C49" s="20">
+        <f>C39-C48</f>
+        <v>0</v>
+      </c>
+      <c r="D49" s="20">
+        <f t="shared" ref="D49:E49" si="11">D39-D48</f>
+        <v>0</v>
+      </c>
+      <c r="E49" s="20">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B49" s="24"/>
-      <c r="C49" s="24">
-        <f>C39-C48</f>
-        <v>0</v>
-      </c>
-      <c r="D49" s="24">
-        <f t="shared" ref="D49:E49" si="11">D39-D48</f>
-        <v>0</v>
-      </c>
-      <c r="E49" s="24">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="F49" s="22"/>
-      <c r="G49" s="22"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="22" t="s">
+      <c r="B50" s="20">
+        <f>ROUND(SUM(C39:E39)-SUM(C48:E48),)</f>
+        <v>0</v>
+      </c>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B50" s="24">
-        <f>ROUND(SUM(C39:E39)-SUM(C48:E48),)</f>
-        <v>0</v>
-      </c>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="22"/>
-      <c r="G50" s="22"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B51" s="24"/>
-      <c r="C51" s="24">
+      <c r="B51" s="20"/>
+      <c r="C51" s="20">
         <f>IF($B$50&gt;0,IF(LARGE($C$49:$F$49,$B$50)&lt;=C$49,1,0), 0)</f>
         <v>0</v>
       </c>
-      <c r="D51" s="24">
-        <f>IF(($B$50-C49)&gt;0,IF(LARGE($C$48:$F$48,$B$44)&lt;=D$49,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E51" s="24">
-        <f>IF(($B$50-SUM($C$49:$D$49))&gt;0,IF(LARGE($C$48:$F$48,$B$44)&lt;=E$49,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F51" s="22"/>
-      <c r="G51" s="22"/>
+      <c r="D51" s="20">
+        <f>IF(($B$50-C49)&gt;0,IF(LARGE($C$49:$F$49,$B$44)&lt;=D$49,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E51" s="20">
+        <f>IF(($B$50-SUM($C$49:$D$49))&gt;0,IF(LARGE($C$49:$F$49,$B$44)&lt;=E$49,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="23" t="s">
+      <c r="A52" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B52" s="19"/>
+      <c r="C52" s="19">
+        <f>C48+C51</f>
+        <v>0</v>
+      </c>
+      <c r="D52" s="19">
+        <f t="shared" ref="D52" si="12">D48+D51</f>
+        <v>295</v>
+      </c>
+      <c r="E52" s="19">
+        <f t="shared" ref="E52" si="13">E48+E51</f>
+        <v>0</v>
+      </c>
+      <c r="F52" s="19"/>
+      <c r="G52" s="19">
+        <f>SUM(C52:E52)</f>
+        <v>295</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B52" s="23"/>
-      <c r="C52" s="23">
-        <f>C48+C51</f>
-        <v>0</v>
-      </c>
-      <c r="D52" s="23">
-        <f t="shared" ref="D52" si="12">D48+D51</f>
-        <v>0</v>
-      </c>
-      <c r="E52" s="23">
-        <f t="shared" ref="E52" si="13">E48+E51</f>
-        <v>0</v>
-      </c>
-      <c r="F52" s="23"/>
-      <c r="G52" s="23">
-        <f>SUM(C52:E52)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="B54" s="23">
+      <c r="B54" s="19">
         <f>G46+G52</f>
-        <v>600</v>
+        <v>1126</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="A18:E19"/>
-    <mergeCell ref="G4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dekningsgrad skal redusere grunnlaget
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling-nyteknking.xlsx
+++ b/doc/okonomi/Utbetaling-nyteknking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/dev/nav/helse-spleis/doc/okonomi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2816A87-78B0-2248-BB57-4C6D4E76A3E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBA44E1-3D04-9D49-ABBF-210317E76F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15560" yWindow="7880" windowWidth="42280" windowHeight="29380" xr2:uid="{D68530E5-53F4-9147-B78C-2EE89FEB1D81}"/>
   </bookViews>
@@ -176,7 +176,7 @@
     <t xml:space="preserve">Totalt utbetalt </t>
   </si>
   <si>
-    <t>Rest som bortfaller pga. dekningsgrad</t>
+    <t>Begrenset grunnlag ihht. Dekningsgrad</t>
   </si>
 </sst>
 </file>
@@ -638,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FF1C860-80D7-1E4E-BCDB-1C6933AA76C9}">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -699,48 +699,40 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="4">
-        <f>MIN(12*SUM(C5:E5),B2)</f>
-        <v>468127.4</v>
-      </c>
-      <c r="C6" s="4"/>
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="4">
+        <f>C5*C7</f>
+        <v>26010.616666666669</v>
+      </c>
+      <c r="D6" s="4">
+        <f>D5*D7</f>
+        <v>6400</v>
+      </c>
+      <c r="E6" s="4">
+        <f>E5*E7</f>
+        <v>5000</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="3">
-        <f>C5/SUM($C$5:$E$5)</f>
-        <v>0.66675738271248386</v>
-      </c>
-      <c r="D7" s="3">
-        <f>D5/SUM($C$5:$E$5)</f>
-        <v>0.20507237986924071</v>
-      </c>
-      <c r="E7" s="3">
-        <f>E5/SUM($C$5:$E$5)</f>
-        <v>0.12817023741827543</v>
+        <v>32</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="8">
-        <f>$B$6*C7/12</f>
-        <v>26010.616666666669</v>
-      </c>
-      <c r="D8" s="8">
-        <f>$B$6*D7/12</f>
-        <v>8000</v>
-      </c>
-      <c r="E8" s="8">
-        <f>$B$6*E7/12</f>
-        <v>4999.9999999999991</v>
-      </c>
-      <c r="F8" t="s">
-        <v>17</v>
+      <c r="B8" s="4">
+        <f>MIN(12*SUM(C6:E6),B2)</f>
+        <v>448927.4</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -748,593 +740,597 @@
         <v>4</v>
       </c>
       <c r="C9" s="3">
-        <f>C8/SUM($C$8:$E$8)</f>
-        <v>0.66675738271248386</v>
+        <f>C6/SUM($C$6:$E$6)</f>
+        <v>0.69527366785809908</v>
       </c>
       <c r="D9" s="3">
-        <f>D8/SUM($C$8:$E$8)</f>
-        <v>0.20507237986924071</v>
+        <f>D6/SUM($C$6:$E$6)</f>
+        <v>0.17107443207966366</v>
       </c>
       <c r="E9" s="3">
-        <f>E8/SUM($C$8:$E$8)</f>
-        <v>0.12817023741827543</v>
-      </c>
-      <c r="F9" t="s">
-        <v>20</v>
+        <f>E6/SUM($C$6:$E$6)</f>
+        <v>0.13365190006223723</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="8">
-        <f>12*SUM(C8:E8)</f>
-        <v>468127.4</v>
-      </c>
-      <c r="C10" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="8">
+        <f>$B$8*C9/12</f>
+        <v>26010.616666666669</v>
+      </c>
+      <c r="D10" s="8">
+        <f>$B$8*D9/12</f>
+        <v>6400</v>
+      </c>
+      <c r="E10" s="8">
+        <f>$B$8*E9/12</f>
+        <v>5000</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3">
+        <f>C10/SUM($C$10:$E$10)</f>
+        <v>0.69527366785809908</v>
+      </c>
+      <c r="D11" s="3">
+        <f>D10/SUM($C$10:$E$10)</f>
+        <v>0.17107443207966366</v>
+      </c>
+      <c r="E11" s="3">
+        <f>E10/SUM($C$10:$E$10)</f>
+        <v>0.13365190006223723</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="8">
+        <f>12*SUM(C10:E10)</f>
+        <v>448927.4</v>
+      </c>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C13" s="11">
         <f>C5</f>
         <v>26010.616666666669</v>
       </c>
-      <c r="D11" s="11">
-        <v>0</v>
-      </c>
-      <c r="E11" s="11">
-        <f t="shared" ref="E11" si="0">E5</f>
+      <c r="D13" s="11">
+        <v>0</v>
+      </c>
+      <c r="E13" s="11">
+        <f>E5</f>
         <v>5000</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="4">
-        <f>12*SUM(C11:E11)</f>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="4">
+        <f>12*SUM(C13:E13)</f>
         <v>372127.4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="2">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="1">
-        <f>MIN(C5,C11)</f>
-        <v>26010.616666666669</v>
-      </c>
-      <c r="D14" s="1">
-        <f t="shared" ref="D14:E14" si="1">MIN(D5,D11)</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="1">
-        <f t="shared" si="1"/>
-        <v>5000</v>
-      </c>
-      <c r="F14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="12">
-        <f>IF(C5&gt;0,C14/C5,0)</f>
-        <v>1</v>
-      </c>
-      <c r="D15" s="12">
-        <f>IF(D5&gt;0,D14/D5,0)</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="12">
-        <f t="shared" ref="D15:E15" si="2">IF(E5&gt;0,E14/E5,0)</f>
-        <v>1</v>
-      </c>
-      <c r="F15" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="1">
+        <f>MIN(C5,C13)</f>
+        <v>26010.616666666669</v>
+      </c>
+      <c r="D16" s="1">
+        <f>MIN(D5,D13)</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <f>MIN(E5,E13)</f>
+        <v>5000</v>
+      </c>
+      <c r="F16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="12">
+        <f>IF(C5&gt;0,C16/C5,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D17" s="12">
+        <f>IF(D5&gt;0,D16/D5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="12">
+        <f>IF(E5&gt;0,E16/E5,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="3">
-        <f>C14/SUM($C$14:$E$14)</f>
+      <c r="C18" s="3">
+        <f>C16/SUM($C$16:$E$16)</f>
         <v>0.83876489610816085</v>
       </c>
-      <c r="D16" s="3">
-        <f t="shared" ref="D16:E16" si="3">D14/SUM($C$14:$E$14)</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="3">
-        <f t="shared" si="3"/>
+      <c r="D18" s="3">
+        <f>D16/SUM($C$16:$E$16)</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <f>E16/SUM($C$16:$E$16)</f>
         <v>0.16123510389183918</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="22" t="s">
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+    </row>
+    <row r="20" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A20" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="13">
-        <f>(C8*C15)/SUMPRODUCT($C$8:$E$8,$C$15:$E$15)</f>
-        <v>0.83876489610816085</v>
-      </c>
-      <c r="D20" s="13">
-        <f>(D8*D15)/SUMPRODUCT($C$8:$E$8,$C$15:$E$15)</f>
-        <v>0</v>
-      </c>
-      <c r="E20" s="13">
-        <f>(E8*E15)/SUMPRODUCT($C$8:$E$8,$C$15:$E$15)</f>
-        <v>0.16123510389183915</v>
-      </c>
-      <c r="F20" t="s">
-        <v>26</v>
-      </c>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="14">
-        <f>(1-C15)</f>
-        <v>0</v>
-      </c>
-      <c r="D21" s="14">
-        <f>(1-D15)</f>
-        <v>1</v>
-      </c>
-      <c r="E21" s="14">
-        <f>(1-E15)</f>
-        <v>0</v>
-      </c>
-      <c r="F21" t="s">
-        <v>26</v>
-      </c>
+      <c r="A21" s="22"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C22" s="13">
-        <f>IF(SUMPRODUCT($C$8:$E$8,$C$21:$E$21)&gt;0,(C8*C21)/SUMPRODUCT($C$8:$E$8,$C$21:$E$21),0)</f>
-        <v>0</v>
+        <f>(C10*C17)/SUMPRODUCT($C$10:$E$10,$C$17:$E$17)</f>
+        <v>0.83876489610816085</v>
       </c>
       <c r="D22" s="13">
-        <f t="shared" ref="D22:E22" si="4">IF(SUMPRODUCT($C$8:$E$8,$C$21:$E$21)&gt;0,(D8*D21)/SUMPRODUCT($C$8:$E$8,$C$21:$E$21),0)</f>
+        <f>(D10*D17)/SUMPRODUCT($C$10:$E$10,$C$17:$E$17)</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="13">
+        <f>(E10*E17)/SUMPRODUCT($C$10:$E$10,$C$17:$E$17)</f>
+        <v>0.16123510389183918</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="14">
+        <f>(1-C17)</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="14">
+        <f>(1-D17)</f>
         <v>1</v>
       </c>
-      <c r="E22" s="13">
-        <f t="shared" si="4"/>
-        <v>0</v>
+      <c r="E23" s="14">
+        <f>(1-E17)</f>
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="13">
+        <f>IF(SUMPRODUCT($C$10:$E$10,$C$23:$E$23)&gt;0,(C10*C23)/SUMPRODUCT($C$10:$E$10,$C$23:$E$23),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="13">
+        <f>IF(SUMPRODUCT($C$10:$E$10,$C$23:$E$23)&gt;0,(D10*D23)/SUMPRODUCT($C$10:$E$10,$C$23:$E$23),0)</f>
+        <v>1</v>
+      </c>
+      <c r="E24" s="13">
+        <f>IF(SUMPRODUCT($C$10:$E$10,$C$23:$E$23)&gt;0,(E10*E23)/SUMPRODUCT($C$10:$E$10,$C$23:$E$23),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C26" s="2">
         <v>0.5</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D26" s="2">
         <v>0.8</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E26" s="2">
         <v>1</v>
       </c>
-      <c r="G24" s="10"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="G26" s="10"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="6">
-        <f>C24*C9</f>
-        <v>0.33337869135624193</v>
-      </c>
-      <c r="D25" s="6">
-        <f>D24*D9</f>
-        <v>0.16405790389539257</v>
-      </c>
-      <c r="E25" s="6">
-        <f>E24*E9</f>
-        <v>0.12817023741827543</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="15">
-        <f>(C20*C24) / SUMPRODUCT($C$20:$E$20,$C$24:$E$24)</f>
-        <v>0.72230411679518591</v>
-      </c>
-      <c r="D27" s="15">
-        <f>(D20*D24) / SUMPRODUCT($C$20:$E$20,$C$24:$E$24)</f>
-        <v>0</v>
-      </c>
-      <c r="E27" s="15">
-        <f>(E20*E24) / SUMPRODUCT($C$20:$E$20,$C$24:$E$24)</f>
-        <v>0.27769588320481409</v>
-      </c>
-      <c r="F27" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" s="3">
-        <f>C11*C24/SUMPRODUCT($C11:$E$11,$C$24:$E$24)</f>
-        <v>0.72230411679518591</v>
-      </c>
-      <c r="D28" s="3">
-        <f>D11*D24/SUMPRODUCT($C11:$E$11,$C$24:$E$24)</f>
-        <v>0</v>
-      </c>
-      <c r="E28" s="3">
-        <f>E11*E24/SUMPRODUCT($C11:$E$11,$C$24:$E$24)</f>
-        <v>0.27769588320481414</v>
-      </c>
-      <c r="F28" t="s">
-        <v>24</v>
+      <c r="C27" s="6">
+        <f>C26*C11</f>
+        <v>0.34763683392904954</v>
+      </c>
+      <c r="D27" s="6">
+        <f>D26*D11</f>
+        <v>0.13685954566373093</v>
+      </c>
+      <c r="E27" s="6">
+        <f>E26*E11</f>
+        <v>0.13365190006223723</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="9"/>
+      <c r="C29" s="15">
+        <f>(C22*C26) / SUMPRODUCT($C$22:$E$22,$C$26:$E$26)</f>
+        <v>0.72230411679518591</v>
+      </c>
+      <c r="D29" s="15">
+        <f>(D22*D26) / SUMPRODUCT($C$22:$E$22,$C$26:$E$26)</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="15">
+        <f>(E22*E26) / SUMPRODUCT($C$22:$E$22,$C$26:$E$26)</f>
+        <v>0.27769588320481414</v>
+      </c>
+      <c r="F29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="3">
+        <f>C13*C26/SUMPRODUCT($C13:$E$13,$C$26:$E$26)</f>
+        <v>0.72230411679518591</v>
+      </c>
+      <c r="D30" s="3">
+        <f>D13*D26/SUMPRODUCT($C13:$E$13,$C$26:$E$26)</f>
+        <v>0</v>
+      </c>
+      <c r="E30" s="3">
+        <f>E13*E26/SUMPRODUCT($C13:$E$13,$C$26:$E$26)</f>
+        <v>0.27769588320481414</v>
+      </c>
+      <c r="F30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="12">
-        <f>IF(SUMPRODUCT($C$22:$E$22,$C$24:$E$24)&gt;0,(C22*C24) / SUMPRODUCT($C$22:$E$22,$C$24:$E$24),0)</f>
-        <v>0</v>
-      </c>
-      <c r="D29" s="12">
-        <f>IF(SUMPRODUCT($C$22:$E$22,$C$24:$E$24)&gt;0,(D22*D24) / SUMPRODUCT($C$22:$E$22,$C$24:$E$24),0)</f>
+      <c r="B31" s="9"/>
+      <c r="C31" s="12">
+        <f>IF(SUMPRODUCT($C$24:$E$24,$C$26:$E$26)&gt;0,(C24*C26) / SUMPRODUCT($C$24:$E$24,$C$26:$E$26),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="12">
+        <f>IF(SUMPRODUCT($C$24:$E$24,$C$26:$E$26)&gt;0,(D24*D26) / SUMPRODUCT($C$24:$E$24,$C$26:$E$26),0)</f>
         <v>1</v>
       </c>
-      <c r="E29" s="12">
-        <f t="shared" ref="E29" si="5">IF(SUMPRODUCT($C$22:$E$22,$C$24:$E$24)&gt;0,(E22*E24) / SUMPRODUCT($C$22:$E$22,$C$24:$E$24),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
+      <c r="E31" s="12">
+        <f>IF(SUMPRODUCT($C$24:$E$24,$C$26:$E$26)&gt;0,(E24*E26) / SUMPRODUCT($C$24:$E$24,$C$26:$E$26),0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" s="16">
-        <f>SUM(C25:E25)</f>
-        <v>0.62560683266991002</v>
-      </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" s="1">
-        <f>ROUND((12*SUMPRODUCT(C8:E8,C24:E24,C15:E15))/260,)*260</f>
-        <v>216060</v>
+        <v>9</v>
+      </c>
+      <c r="B33" s="16">
+        <f>SUM(C27:E27)</f>
+        <v>0.61814827965501773</v>
       </c>
       <c r="C33" s="1"/>
-      <c r="D33" s="3"/>
-      <c r="F33" t="s">
-        <v>39</v>
-      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="4">
-        <f>ROUND(B10*B32/260,)*260</f>
-        <v>292760</v>
-      </c>
-      <c r="C34" s="4">
-        <f>B34/260</f>
-        <v>1126</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B34" s="1">
+        <f>ROUND((12*SUMPRODUCT(C10:E10,C26:E26,C17:E17))/260,)*260</f>
+        <v>216060</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="3"/>
       <c r="F34" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B35" s="4">
-        <f>MIN(B33,B34)</f>
-        <v>216060</v>
+        <f>ROUND(B12*B33/260,)*260</f>
+        <v>277420</v>
+      </c>
+      <c r="C35" s="4">
+        <f>B35/260</f>
+        <v>1067</v>
+      </c>
+      <c r="F35" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="4">
+        <f>MIN(B34,B35)</f>
+        <v>216060</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="4">
-        <f>B34-B35</f>
-        <v>76700</v>
-      </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C37" s="4"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="4"/>
+      <c r="B37" s="4">
+        <f>B35-B36</f>
+        <v>61360</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="23">
-        <f>$B$35*C27/260*C13</f>
-        <v>600.23472105679957</v>
-      </c>
-      <c r="D38" s="23">
-        <f t="shared" ref="D38:E38" si="6">$B$35*D27/260*D13</f>
-        <v>0</v>
-      </c>
-      <c r="E38" s="23">
-        <f t="shared" si="6"/>
-        <v>230.76527894320049</v>
-      </c>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18">
-        <f>SUM(C38:E38)</f>
-        <v>831</v>
-      </c>
+      <c r="C38" s="4"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="4"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="18" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B39" s="18"/>
       <c r="C39" s="23">
-        <f>$B$36*C29/260*C13</f>
-        <v>0</v>
+        <f>$B$36*C29/260</f>
+        <v>600.23472105679957</v>
       </c>
       <c r="D39" s="23">
-        <f t="shared" ref="D39:E39" si="7">$B$36*D29/260*D13</f>
-        <v>236</v>
+        <f t="shared" ref="D39:E39" si="0">$B$36*D29/260</f>
+        <v>0</v>
       </c>
       <c r="E39" s="23">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>230.76527894320054</v>
       </c>
       <c r="F39" s="18"/>
       <c r="G39" s="18">
         <f>SUM(C39:E39)</f>
+        <v>831.00000000000011</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="18"/>
+      <c r="C40" s="23">
+        <f>$B$37*C31/260</f>
+        <v>0</v>
+      </c>
+      <c r="D40" s="23">
+        <f t="shared" ref="D40:E40" si="1">$B$37*D31/260</f>
         <v>236</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="18"/>
-      <c r="B40" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40" s="20">
-        <f>SUM(C38:C39)</f>
-        <v>600.23472105679957</v>
-      </c>
-      <c r="D40" s="20">
-        <f t="shared" ref="D40:E40" si="8">SUM(D38:D39)</f>
-        <v>236</v>
-      </c>
-      <c r="E40" s="20">
-        <f t="shared" si="8"/>
-        <v>230.76527894320049</v>
+      <c r="E40" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="F40" s="18"/>
       <c r="G40" s="18">
-        <f>SUM(G38:G39)</f>
-        <v>1067</v>
+        <f>SUM(C40:E40)</f>
+        <v>236</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="18"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
+      <c r="B41" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" s="20">
+        <f>SUM(C39:C40)</f>
+        <v>600.23472105679957</v>
+      </c>
+      <c r="D41" s="20">
+        <f t="shared" ref="D41:E41" si="2">SUM(D39:D40)</f>
+        <v>236</v>
+      </c>
+      <c r="E41" s="20">
+        <f t="shared" si="2"/>
+        <v>230.76527894320054</v>
+      </c>
       <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
+      <c r="G41" s="18">
+        <f>SUM(G39:G40)</f>
+        <v>1067</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="18" t="s">
-        <v>11</v>
-      </c>
+      <c r="A42" s="18"/>
       <c r="B42" s="18"/>
-      <c r="C42" s="20">
-        <f>TRUNC(C38)</f>
-        <v>600</v>
-      </c>
-      <c r="D42" s="20">
-        <f t="shared" ref="D42:E42" si="9">TRUNC(D38)</f>
-        <v>0</v>
-      </c>
-      <c r="E42" s="20">
-        <f t="shared" si="9"/>
-        <v>230</v>
-      </c>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
       <c r="F42" s="18"/>
       <c r="G42" s="18"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="18" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B43" s="18"/>
       <c r="C43" s="20">
-        <f>C38-C42</f>
-        <v>0.23472105679957167</v>
+        <f>TRUNC(C39)</f>
+        <v>600</v>
       </c>
       <c r="D43" s="20">
-        <f t="shared" ref="D43:E43" si="10">D38-D42</f>
+        <f t="shared" ref="D43:E43" si="3">TRUNC(D39)</f>
         <v>0</v>
       </c>
       <c r="E43" s="20">
-        <f t="shared" si="10"/>
-        <v>0.76527894320048517</v>
+        <f t="shared" si="3"/>
+        <v>230</v>
       </c>
       <c r="F43" s="18"/>
       <c r="G43" s="18"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B44" s="20">
-        <f>ROUND(SUM(C38:E38)-SUM(C42:E42),)</f>
-        <v>1</v>
-      </c>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
+        <v>40</v>
+      </c>
+      <c r="B44" s="18"/>
+      <c r="C44" s="20">
+        <f>C39-C43</f>
+        <v>0.23472105679957167</v>
+      </c>
+      <c r="D44" s="20">
+        <f t="shared" ref="D44:E44" si="4">D39-D43</f>
+        <v>0</v>
+      </c>
+      <c r="E44" s="20">
+        <f t="shared" si="4"/>
+        <v>0.76527894320054202</v>
+      </c>
       <c r="F44" s="18"/>
       <c r="G44" s="18"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="20">
-        <f>IF($B$44&gt;0,IF(LARGE($C$43:$F$43,$B$44)&lt;=C$43,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D45" s="20">
-        <f>IF(($B$44-C45)&gt;0,IF(LARGE($C$43:$F$43,$B$44)&lt;=D$43,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E45" s="20">
-        <f>IF(($B$44-SUM($C$45:$D$45))&gt;0,IF(LARGE($C$43:$F$43,$B$44)&lt;=E$43,1,0), 0)</f>
+        <v>41</v>
+      </c>
+      <c r="B45" s="20">
+        <f>ROUND(SUM(C39:E39)-SUM(C43:E43),)</f>
         <v>1</v>
       </c>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
       <c r="F45" s="18"/>
       <c r="G45" s="18"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="19" t="s">
+      <c r="A46" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" s="18"/>
+      <c r="C46" s="20">
+        <f>IF($B$45&gt;0,IF(LARGE($C$44:$F$44,$B$45)&lt;=C$44,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D46" s="20">
+        <f>IF(($B$45-C46)&gt;0,IF(LARGE($C$44:$F$44,$B$45)&lt;=D$44,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E46" s="20">
+        <f>IF(($B$45-SUM($C$46:$D$46))&gt;0,IF(LARGE($C$44:$F$44,$B$45)&lt;=E$44,1,0), 0)</f>
+        <v>1</v>
+      </c>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19">
-        <f>C42+C45</f>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19">
+        <f>C43+C46</f>
         <v>600</v>
       </c>
-      <c r="D46" s="19">
-        <f t="shared" ref="D46:E46" si="11">D42+D45</f>
-        <v>0</v>
-      </c>
-      <c r="E46" s="19">
-        <f t="shared" si="11"/>
+      <c r="D47" s="19">
+        <f t="shared" ref="D47:E47" si="5">D43+D46</f>
+        <v>0</v>
+      </c>
+      <c r="E47" s="19">
+        <f t="shared" si="5"/>
         <v>231</v>
       </c>
-      <c r="F46" s="19"/>
-      <c r="G46" s="19">
-        <f>SUM(C46:E46)</f>
+      <c r="F47" s="19"/>
+      <c r="G47" s="19">
+        <f>SUM(C47:E47)</f>
         <v>831</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="18"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-    </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="18" t="s">
-        <v>19</v>
-      </c>
+      <c r="A48" s="18"/>
       <c r="B48" s="20"/>
-      <c r="C48" s="20">
-        <f>TRUNC(C39)</f>
-        <v>0</v>
-      </c>
-      <c r="D48" s="20">
-        <f t="shared" ref="D48:E48" si="12">TRUNC(D39)</f>
-        <v>236</v>
-      </c>
-      <c r="E48" s="20">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
       <c r="F48" s="18"/>
       <c r="G48" s="18"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="18" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="B49" s="20"/>
       <c r="C49" s="20">
-        <f>C39-C48</f>
+        <f>TRUNC(C40)</f>
         <v>0</v>
       </c>
       <c r="D49" s="20">
-        <f t="shared" ref="D49:E49" si="13">D39-D48</f>
-        <v>0</v>
+        <f t="shared" ref="D49:E49" si="6">TRUNC(D40)</f>
+        <v>236</v>
       </c>
       <c r="E49" s="20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F49" s="18"/>
@@ -1342,84 +1338,94 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B50" s="20">
-        <f>ROUND(SUM(C39:E39)-SUM(C48:E48),)</f>
-        <v>0</v>
-      </c>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
+        <v>40</v>
+      </c>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20">
+        <f>C40-C49</f>
+        <v>0</v>
+      </c>
+      <c r="D50" s="20">
+        <f t="shared" ref="D50:E50" si="7">D40-D49</f>
+        <v>0</v>
+      </c>
+      <c r="E50" s="20">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
       <c r="F50" s="18"/>
       <c r="G50" s="18"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20">
-        <f>IF($B$50&gt;0,IF(LARGE($C$49:$F$49,$B$50)&lt;=C$49,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D51" s="20">
-        <f>IF(($B$50-C49)&gt;0,IF(LARGE($C$49:$F$49,$B$44)&lt;=D$49,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E51" s="20">
-        <f>IF(($B$50-SUM($C$49:$D$49))&gt;0,IF(LARGE($C$49:$F$49,$B$44)&lt;=E$49,1,0), 0)</f>
-        <v>0</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="B51" s="20">
+        <f>ROUND(SUM(C40:E40)-SUM(C49:E49),)</f>
+        <v>0</v>
+      </c>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
       <c r="F51" s="18"/>
       <c r="G51" s="18"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="19" t="s">
+      <c r="A52" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" s="20"/>
+      <c r="C52" s="20">
+        <f>IF($B$51&gt;0,IF(LARGE($C$50:$F$50,$B$51)&lt;=C$50,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D52" s="20">
+        <f>IF(($B$51-C50)&gt;0,IF(LARGE($C$50:$F$50,$B$45)&lt;=D$50,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E52" s="20">
+        <f>IF(($B$51-SUM($C$50:$D$50))&gt;0,IF(LARGE($C$50:$F$50,$B$45)&lt;=E$50,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B52" s="19"/>
-      <c r="C52" s="19">
-        <f>C48+C51</f>
-        <v>0</v>
-      </c>
-      <c r="D52" s="19">
-        <f t="shared" ref="D52" si="14">D48+D51</f>
+      <c r="B53" s="19"/>
+      <c r="C53" s="19">
+        <f>C49+C52</f>
+        <v>0</v>
+      </c>
+      <c r="D53" s="19">
+        <f t="shared" ref="D53" si="8">D49+D52</f>
         <v>236</v>
       </c>
-      <c r="E52" s="19">
-        <f t="shared" ref="E52" si="15">E48+E51</f>
-        <v>0</v>
-      </c>
-      <c r="F52" s="19"/>
-      <c r="G52" s="19">
-        <f>SUM(C52:E52)</f>
+      <c r="E53" s="19">
+        <f t="shared" ref="E53" si="9">E49+E52</f>
+        <v>0</v>
+      </c>
+      <c r="F53" s="19"/>
+      <c r="G53" s="19">
+        <f>SUM(C53:E53)</f>
         <v>236</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="19" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B54" s="19">
-        <f>G46+G52</f>
+      <c r="B55" s="19">
+        <f>G47+G53</f>
         <v>1067</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>46</v>
-      </c>
-      <c r="B55" s="4">
-        <f>C34-B54</f>
-        <v>59</v>
-      </c>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B56" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A18:E19"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
setter opp et eksempel
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling-nyteknking.xlsx
+++ b/doc/okonomi/Utbetaling-nyteknking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/dev/nav/helse-spleis/doc/okonomi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBA44E1-3D04-9D49-ABBF-210317E76F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E483CC8-4854-6743-810B-A399C34E2A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15560" yWindow="7880" windowWidth="42280" windowHeight="29380" xr2:uid="{D68530E5-53F4-9147-B78C-2EE89FEB1D81}"/>
+    <workbookView xWindow="6320" yWindow="2860" windowWidth="58300" windowHeight="38640" xr2:uid="{D68530E5-53F4-9147-B78C-2EE89FEB1D81}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
   <si>
     <t>Månedsinntekt</t>
   </si>
@@ -177,16 +177,27 @@
   </si>
   <si>
     <t>Begrenset grunnlag ihht. Dekningsgrad</t>
+  </si>
+  <si>
+    <t>Avrundet Sykepengegrunnlag</t>
+  </si>
+  <si>
+    <t>Samlet refusjonsgrad</t>
+  </si>
+  <si>
+    <t>Refusjon gitt 100 % syk</t>
+  </si>
+  <si>
+    <t>Personbeløp gitt 100 % syk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;NOK&quot;\ * #,##0.00_-;\-&quot;NOK&quot;\ * #,##0.00_-;_-&quot;NOK&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0000%"/>
-    <numFmt numFmtId="165" formatCode="0.00000%"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -293,7 +304,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -311,17 +322,16 @@
     <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -638,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FF1C860-80D7-1E4E-BCDB-1C6933AA76C9}">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -652,10 +662,11 @@
     <col min="4" max="4" width="20.33203125" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
+    <col min="8" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -663,7 +674,7 @@
         <v>93634</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -672,7 +683,7 @@
         <v>561804</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
@@ -683,39 +694,40 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="1">
-        <f>1200.49*260/12</f>
-        <v>26010.616666666669</v>
+        <v>15000</v>
       </c>
       <c r="D5" s="1">
-        <v>8000</v>
+        <v>500</v>
       </c>
       <c r="E5" s="1">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>46</v>
       </c>
       <c r="C6" s="4">
         <f>C5*C7</f>
-        <v>26010.616666666669</v>
+        <v>15000</v>
       </c>
       <c r="D6" s="4">
         <f>D5*D7</f>
-        <v>6400</v>
+        <v>500</v>
       </c>
       <c r="E6" s="4">
         <f>E5*E7</f>
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -723,123 +735,122 @@
         <v>1</v>
       </c>
       <c r="D7" s="2">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" s="4">
         <f>MIN(12*SUM(C6:E6),B2)</f>
-        <v>448927.4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>186000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="3">
         <f>C6/SUM($C$6:$E$6)</f>
-        <v>0.69527366785809908</v>
+        <v>0.967741935483871</v>
       </c>
       <c r="D9" s="3">
         <f>D6/SUM($C$6:$E$6)</f>
-        <v>0.17107443207966366</v>
+        <v>3.2258064516129031E-2</v>
       </c>
       <c r="E9" s="3">
         <f>E6/SUM($C$6:$E$6)</f>
-        <v>0.13365190006223723</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="8">
         <f>$B$8*C9/12</f>
-        <v>26010.616666666669</v>
+        <v>15000</v>
       </c>
       <c r="D10" s="8">
         <f>$B$8*D9/12</f>
-        <v>6400</v>
+        <v>500</v>
       </c>
       <c r="E10" s="8">
         <f>$B$8*E9/12</f>
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="F10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="3">
         <f>C10/SUM($C$10:$E$10)</f>
-        <v>0.69527366785809908</v>
+        <v>0.967741935483871</v>
       </c>
       <c r="D11" s="3">
         <f>D10/SUM($C$10:$E$10)</f>
-        <v>0.17107443207966366</v>
+        <v>3.2258064516129031E-2</v>
       </c>
       <c r="E11" s="3">
         <f>E10/SUM($C$10:$E$10)</f>
-        <v>0.13365190006223723</v>
+        <v>0</v>
       </c>
       <c r="F11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="8">
         <f>12*SUM(C10:E10)</f>
-        <v>448927.4</v>
+        <v>186000</v>
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="11">
-        <f>C5</f>
-        <v>26010.616666666669</v>
+        <v>14999</v>
       </c>
       <c r="D13" s="11">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="E13" s="11">
         <f>E5</f>
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="4">
         <f>12*SUM(C13:E13)</f>
-        <v>372127.4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>181428</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="1">
         <f>MIN(C5,C13)</f>
-        <v>26010.616666666669</v>
+        <v>14999</v>
       </c>
       <c r="D16" s="1">
         <f>MIN(D5,D13)</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="E16" s="1">
         <f>MIN(E5,E13)</f>
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="F16" t="s">
         <v>31</v>
@@ -852,15 +863,15 @@
       <c r="B17" s="9"/>
       <c r="C17" s="12">
         <f>IF(C5&gt;0,C16/C5,0)</f>
-        <v>1</v>
+        <v>0.99993333333333334</v>
       </c>
       <c r="D17" s="12">
         <f>IF(D5&gt;0,D16/D5,0)</f>
-        <v>0</v>
+        <v>0.24</v>
       </c>
       <c r="E17" s="12">
         <f>IF(E5&gt;0,E16/E5,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" t="s">
         <v>38</v>
@@ -872,15 +883,15 @@
       </c>
       <c r="C18" s="3">
         <f>C16/SUM($C$16:$E$16)</f>
-        <v>0.83876489610816085</v>
+        <v>0.99206296712745556</v>
       </c>
       <c r="D18" s="3">
         <f>D16/SUM($C$16:$E$16)</f>
-        <v>0</v>
+        <v>7.9370328725444812E-3</v>
       </c>
       <c r="E18" s="3">
         <f>E16/SUM($C$16:$E$16)</f>
-        <v>0.16123510389183918</v>
+        <v>0</v>
       </c>
       <c r="F18" t="s">
         <v>36</v>
@@ -895,7 +906,7 @@
       <c r="D19" s="21"/>
       <c r="E19" s="21"/>
     </row>
-    <row r="20" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
         <v>37</v>
       </c>
@@ -913,519 +924,557 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="13">
-        <f>(C10*C17)/SUMPRODUCT($C$10:$E$10,$C$17:$E$17)</f>
-        <v>0.83876489610816085</v>
-      </c>
-      <c r="D22" s="13">
-        <f>(D10*D17)/SUMPRODUCT($C$10:$E$10,$C$17:$E$17)</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="13">
-        <f>(E10*E17)/SUMPRODUCT($C$10:$E$10,$C$17:$E$17)</f>
-        <v>0.16123510389183918</v>
-      </c>
-      <c r="F22" t="s">
-        <v>26</v>
+        <v>49</v>
+      </c>
+      <c r="B22" s="1">
+        <f>SUMPRODUCT($C$10:$E$10,$C$17:$E$17)</f>
+        <v>15119</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="14">
-        <f>(1-C17)</f>
-        <v>0</v>
-      </c>
-      <c r="D23" s="14">
-        <f>(1-D17)</f>
-        <v>1</v>
-      </c>
-      <c r="E23" s="14">
-        <f>(1-E17)</f>
-        <v>0</v>
-      </c>
-      <c r="F23" t="s">
-        <v>26</v>
+        <v>50</v>
+      </c>
+      <c r="B23" s="1">
+        <f>SUMPRODUCT($C$10:$E$10,$C$25:$E$25)</f>
+        <v>380.99999999999989</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C24" s="13">
-        <f>IF(SUMPRODUCT($C$10:$E$10,$C$23:$E$23)&gt;0,(C10*C23)/SUMPRODUCT($C$10:$E$10,$C$23:$E$23),0)</f>
-        <v>0</v>
+        <f>C10*C17/$B$22</f>
+        <v>0.99206296712745556</v>
       </c>
       <c r="D24" s="13">
-        <f>IF(SUMPRODUCT($C$10:$E$10,$C$23:$E$23)&gt;0,(D10*D23)/SUMPRODUCT($C$10:$E$10,$C$23:$E$23),0)</f>
+        <f>D10*D17/$B$22</f>
+        <v>7.9370328725444812E-3</v>
+      </c>
+      <c r="E24" s="13">
+        <f>E10*E17/$B$22</f>
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="14">
+        <f>(1-C17)</f>
+        <v>6.6666666666659324E-5</v>
+      </c>
+      <c r="D25" s="14">
+        <f>(1-D17)</f>
+        <v>0.76</v>
+      </c>
+      <c r="E25" s="14">
+        <f>(1-E17)</f>
         <v>1</v>
       </c>
-      <c r="E24" s="13">
-        <f>IF(SUMPRODUCT($C$10:$E$10,$C$23:$E$23)&gt;0,(E10*E23)/SUMPRODUCT($C$10:$E$10,$C$23:$E$23),0)</f>
-        <v>0</v>
+      <c r="F25" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="13">
+        <f>IF(SUMPRODUCT($C$10:$E$10,$C$25:$E$25)&gt;0,(C10*C25)/$B$23,0)</f>
+        <v>2.6246719160102103E-3</v>
+      </c>
+      <c r="D26" s="13">
+        <f t="shared" ref="D26:E26" si="0">IF(SUMPRODUCT($C$10:$E$10,$C$25:$E$25)&gt;0,(D10*D25)/$B$23,0)</f>
+        <v>0.99737532808398977</v>
+      </c>
+      <c r="E26" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D26" s="2">
+      <c r="C28" s="2">
         <v>0.8</v>
       </c>
-      <c r="E26" s="2">
+      <c r="D28" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="E28" s="2">
         <v>1</v>
       </c>
-      <c r="G26" s="10"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="6">
-        <f>C26*C11</f>
-        <v>0.34763683392904954</v>
-      </c>
-      <c r="D27" s="6">
-        <f>D26*D11</f>
-        <v>0.13685954566373093</v>
-      </c>
-      <c r="E27" s="6">
-        <f>E26*E11</f>
-        <v>0.13365190006223723</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="15">
-        <f>(C22*C26) / SUMPRODUCT($C$22:$E$22,$C$26:$E$26)</f>
-        <v>0.72230411679518591</v>
-      </c>
-      <c r="D29" s="15">
-        <f>(D22*D26) / SUMPRODUCT($C$22:$E$22,$C$26:$E$26)</f>
-        <v>0</v>
-      </c>
-      <c r="E29" s="15">
-        <f>(E22*E26) / SUMPRODUCT($C$22:$E$22,$C$26:$E$26)</f>
-        <v>0.27769588320481414</v>
-      </c>
-      <c r="F29" t="s">
-        <v>18</v>
-      </c>
+      <c r="C29" s="6">
+        <f>C28*C11</f>
+        <v>0.77419354838709686</v>
+      </c>
+      <c r="D29" s="6">
+        <f>D28*D11</f>
+        <v>2.4193548387096774E-2</v>
+      </c>
+      <c r="E29" s="6">
+        <f>E28*E11</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="4"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="3">
-        <f>C13*C26/SUMPRODUCT($C13:$E$13,$C$26:$E$26)</f>
-        <v>0.72230411679518591</v>
-      </c>
-      <c r="D30" s="3">
-        <f>D13*D26/SUMPRODUCT($C13:$E$13,$C$26:$E$26)</f>
-        <v>0</v>
-      </c>
-      <c r="E30" s="3">
-        <f>E13*E26/SUMPRODUCT($C13:$E$13,$C$26:$E$26)</f>
-        <v>0.27769588320481414</v>
-      </c>
-      <c r="F30" t="s">
-        <v>24</v>
-      </c>
+      <c r="C30" s="4"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="9"/>
+      <c r="C31" s="15">
+        <f>C24*C28 / SUMPRODUCT($C$24:$E$24,$C$28:$E$28)</f>
+        <v>0.99255533864937295</v>
+      </c>
+      <c r="D31" s="15">
+        <f>D24*D28 / SUMPRODUCT($C$24:$E$24,$C$28:$E$28)</f>
+        <v>7.4446613506270066E-3</v>
+      </c>
+      <c r="E31" s="15">
+        <f>E24*E28 / SUMPRODUCT($C$24:$E$24,$C$28:$E$28)</f>
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="3">
+        <f>C11*C13*C28/SUMPRODUCT($C13:$E$13,$C$28:$E$28,$C$11:$E$11)</f>
+        <v>0.99975004582493221</v>
+      </c>
+      <c r="D32" s="3">
+        <f>D11*D13*D28/SUMPRODUCT($C13:$E$13,$C$28:$E$28,$C$11:$E$11)</f>
+        <v>2.4995417506790422E-4</v>
+      </c>
+      <c r="E32" s="3">
+        <f>E11*E13*E28/SUMPRODUCT($C13:$E$13,$C$28:$E$28,$C$11:$E$11)</f>
+        <v>0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="12">
-        <f>IF(SUMPRODUCT($C$24:$E$24,$C$26:$E$26)&gt;0,(C24*C26) / SUMPRODUCT($C$24:$E$24,$C$26:$E$26),0)</f>
-        <v>0</v>
-      </c>
-      <c r="D31" s="12">
-        <f>IF(SUMPRODUCT($C$24:$E$24,$C$26:$E$26)&gt;0,(D24*D26) / SUMPRODUCT($C$24:$E$24,$C$26:$E$26),0)</f>
-        <v>1</v>
-      </c>
-      <c r="E31" s="12">
-        <f>IF(SUMPRODUCT($C$24:$E$24,$C$26:$E$26)&gt;0,(E24*E26) / SUMPRODUCT($C$24:$E$24,$C$26:$E$26),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>9</v>
-      </c>
-      <c r="B33" s="16">
-        <f>SUM(C27:E27)</f>
-        <v>0.61814827965501773</v>
-      </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="12">
+        <f>IF(SUMPRODUCT($C$26:$E$26,$C$28:$E$28)&gt;0,(C26*C28) / SUMPRODUCT($C$26:$E$26,$C$28:$E$28),0)</f>
+        <v>2.7991602519241154E-3</v>
+      </c>
+      <c r="D33" s="12">
+        <f>IF(SUMPRODUCT($C$26:$E$26,$C$28:$E$28)&gt;0,(D26*D28) / SUMPRODUCT($C$26:$E$26,$C$28:$E$28),0)</f>
+        <v>0.99720083974807594</v>
+      </c>
+      <c r="E33" s="12">
+        <f>IF(SUMPRODUCT($C$26:$E$26,$C$28:$E$28)&gt;0,(E26*E28) / SUMPRODUCT($C$26:$E$26,$C$28:$E$28),0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B34" s="1">
-        <f>ROUND((12*SUMPRODUCT(C10:E10,C26:E26,C17:E17))/260,)*260</f>
-        <v>216060</v>
-      </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="3"/>
-      <c r="F34" t="s">
-        <v>39</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B34" s="16">
+        <f>SUM(C29:E29)</f>
+        <v>0.79838709677419362</v>
+      </c>
+      <c r="E34" s="4"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="4">
-        <f>ROUND(B12*B33/260,)*260</f>
-        <v>277420</v>
-      </c>
-      <c r="C35" s="4">
-        <f>B35/260</f>
-        <v>1067</v>
-      </c>
-      <c r="F35" t="s">
-        <v>39</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="B35" s="6">
+        <f>B36/B37</f>
+        <v>0.97690505050505061</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" s="4">
-        <f>MIN(B34,B35)</f>
-        <v>216060</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B36" s="1">
+        <f>12*SUMPRODUCT(C10:E10,C28:E28,C17:E17)</f>
+        <v>145070.40000000002</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="4">
+        <f>B12*B34</f>
+        <v>148500</v>
+      </c>
+      <c r="C37" s="4">
+        <f>B37/260</f>
+        <v>571.15384615384619</v>
+      </c>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="4">
+        <f>ROUND(B37/260,)*260</f>
+        <v>148460</v>
+      </c>
+      <c r="C38" s="4">
+        <f>B38/260</f>
+        <v>571</v>
+      </c>
+      <c r="F38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" s="4">
+        <f>B38*B35</f>
+        <v>145031.3237979798</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="4">
-        <f>B35-B36</f>
-        <v>61360</v>
-      </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C38" s="4"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="4"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="18" t="s">
+      <c r="B40" s="4">
+        <f>B38-B39</f>
+        <v>3428.6762020202004</v>
+      </c>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="23">
-        <f>$B$36*C29/260</f>
-        <v>600.23472105679957</v>
-      </c>
-      <c r="D39" s="23">
-        <f t="shared" ref="D39:E39" si="0">$B$36*D29/260</f>
-        <v>0</v>
-      </c>
-      <c r="E39" s="23">
-        <f t="shared" si="0"/>
-        <v>230.76527894320054</v>
-      </c>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18">
-        <f>SUM(C39:E39)</f>
-        <v>831.00000000000011</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="18" t="s">
+      <c r="B41" s="17"/>
+      <c r="C41" s="20">
+        <f>$B$39*C31/260</f>
+        <v>553.66005656565653</v>
+      </c>
+      <c r="D41" s="20">
+        <f>$B$39*D31/260</f>
+        <v>4.1527272727272733</v>
+      </c>
+      <c r="E41" s="20">
+        <f>$B$39*E31/260</f>
+        <v>0</v>
+      </c>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17">
+        <f>SUM(C41:E41)</f>
+        <v>557.81278383838378</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="23">
-        <f>$B$37*C31/260</f>
-        <v>0</v>
-      </c>
-      <c r="D40" s="23">
-        <f t="shared" ref="D40:E40" si="1">$B$37*D31/260</f>
-        <v>236</v>
-      </c>
-      <c r="E40" s="23">
+      <c r="B42" s="17"/>
+      <c r="C42" s="20">
+        <f>$B$40*C33/260</f>
+        <v>3.6913131313127241E-2</v>
+      </c>
+      <c r="D42" s="20">
+        <f>$B$40*D33/260</f>
+        <v>13.150303030303029</v>
+      </c>
+      <c r="E42" s="20">
+        <f>$B$40*E33/260</f>
+        <v>0</v>
+      </c>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17">
+        <f>SUM(C42:E42)</f>
+        <v>13.187216161616156</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="17"/>
+      <c r="B43" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" s="19">
+        <f>SUM(C41:C42)</f>
+        <v>553.69696969696963</v>
+      </c>
+      <c r="D43" s="19">
+        <f t="shared" ref="D43:E43" si="1">SUM(D41:D42)</f>
+        <v>17.303030303030301</v>
+      </c>
+      <c r="E43" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18">
-        <f>SUM(C40:E40)</f>
-        <v>236</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="18"/>
-      <c r="B41" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C41" s="20">
-        <f>SUM(C39:C40)</f>
-        <v>600.23472105679957</v>
-      </c>
-      <c r="D41" s="20">
-        <f t="shared" ref="D41:E41" si="2">SUM(D39:D40)</f>
-        <v>236</v>
-      </c>
-      <c r="E41" s="20">
+      <c r="F43" s="17"/>
+      <c r="G43" s="17">
+        <f>SUM(G41:G42)</f>
+        <v>570.99999999999989</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="17"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" s="17"/>
+      <c r="C45" s="19">
+        <f>TRUNC(C41)</f>
+        <v>553</v>
+      </c>
+      <c r="D45" s="19">
+        <f t="shared" ref="D45:E45" si="2">TRUNC(D41)</f>
+        <v>4</v>
+      </c>
+      <c r="E45" s="19">
         <f t="shared" si="2"/>
-        <v>230.76527894320054</v>
-      </c>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18">
-        <f>SUM(G39:G40)</f>
-        <v>1067</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="18"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="20">
-        <f>TRUNC(C39)</f>
-        <v>600</v>
-      </c>
-      <c r="D43" s="20">
-        <f t="shared" ref="D43:E43" si="3">TRUNC(D39)</f>
-        <v>0</v>
-      </c>
-      <c r="E43" s="20">
+        <v>0</v>
+      </c>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" s="17"/>
+      <c r="C46" s="19">
+        <f>C41-C45</f>
+        <v>0.66005656565653226</v>
+      </c>
+      <c r="D46" s="19">
+        <f t="shared" ref="D46:E46" si="3">D41-D45</f>
+        <v>0.15272727272727327</v>
+      </c>
+      <c r="E46" s="19">
         <f t="shared" si="3"/>
-        <v>230</v>
-      </c>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="20">
-        <f>C39-C43</f>
-        <v>0.23472105679957167</v>
-      </c>
-      <c r="D44" s="20">
-        <f t="shared" ref="D44:E44" si="4">D39-D43</f>
-        <v>0</v>
-      </c>
-      <c r="E44" s="20">
-        <f t="shared" si="4"/>
-        <v>0.76527894320054202</v>
-      </c>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B45" s="20">
-        <f>ROUND(SUM(C39:E39)-SUM(C43:E43),)</f>
+      <c r="B47" s="20">
+        <f>ROUND(SUM(C41:E41)-SUM(C45:E45),)</f>
         <v>1</v>
       </c>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="18" t="s">
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B46" s="18"/>
-      <c r="C46" s="20">
-        <f>IF($B$45&gt;0,IF(LARGE($C$44:$F$44,$B$45)&lt;=C$44,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D46" s="20">
-        <f>IF(($B$45-C46)&gt;0,IF(LARGE($C$44:$F$44,$B$45)&lt;=D$44,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E46" s="20">
-        <f>IF(($B$45-SUM($C$46:$D$46))&gt;0,IF(LARGE($C$44:$F$44,$B$45)&lt;=E$44,1,0), 0)</f>
+      <c r="B48" s="17"/>
+      <c r="C48" s="19">
+        <f>IF($B$47&gt;0,IF(LARGE($C$46:$F$46,$B$47)&lt;=C$46,1,0), 0)</f>
         <v>1</v>
       </c>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B47" s="19"/>
-      <c r="C47" s="19">
-        <f>C43+C46</f>
-        <v>600</v>
-      </c>
-      <c r="D47" s="19">
-        <f t="shared" ref="D47:E47" si="5">D43+D46</f>
-        <v>0</v>
-      </c>
-      <c r="E47" s="19">
-        <f t="shared" si="5"/>
-        <v>231</v>
-      </c>
-      <c r="F47" s="19"/>
-      <c r="G47" s="19">
-        <f>SUM(C47:E47)</f>
-        <v>831</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="18"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="D48" s="19">
+        <f>IF(($B$47-C48)&gt;0,IF(LARGE($C$46:$F$46,$B$47)&lt;=D$46,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E48" s="19">
+        <f>IF(($B$47-SUM($C$48:$D$48))&gt;0,IF(LARGE($C$46:$F$46,$B$47)&lt;=E$46,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49" s="18"/>
+      <c r="C49" s="18">
+        <f>C45+C48</f>
+        <v>554</v>
+      </c>
+      <c r="D49" s="18">
+        <f t="shared" ref="D49:E49" si="4">D45+D48</f>
+        <v>4</v>
+      </c>
+      <c r="E49" s="18">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18">
+        <f>SUM(C49:E49)</f>
+        <v>558</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="17"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B49" s="20"/>
-      <c r="C49" s="20">
-        <f>TRUNC(C40)</f>
-        <v>0</v>
-      </c>
-      <c r="D49" s="20">
-        <f t="shared" ref="D49:E49" si="6">TRUNC(D40)</f>
-        <v>236</v>
-      </c>
-      <c r="E49" s="20">
+      <c r="B51" s="19"/>
+      <c r="C51" s="20">
+        <f>TRUNC(C42)</f>
+        <v>0</v>
+      </c>
+      <c r="D51" s="19">
+        <f t="shared" ref="D51:E51" si="5">TRUNC(D42)</f>
+        <v>13</v>
+      </c>
+      <c r="E51" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B52" s="19"/>
+      <c r="C52" s="19">
+        <f>C42-C51</f>
+        <v>3.6913131313127241E-2</v>
+      </c>
+      <c r="D52" s="19">
+        <f t="shared" ref="D52:E52" si="6">D42-D51</f>
+        <v>0.15030303030302861</v>
+      </c>
+      <c r="E52" s="19">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F49" s="18"/>
-      <c r="G49" s="18"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20">
-        <f>C40-C49</f>
-        <v>0</v>
-      </c>
-      <c r="D50" s="20">
-        <f t="shared" ref="D50:E50" si="7">D40-D49</f>
-        <v>0</v>
-      </c>
-      <c r="E50" s="20">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="F50" s="18"/>
-      <c r="G50" s="18"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="18" t="s">
+      <c r="F52" s="17"/>
+      <c r="G52" s="17"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B51" s="20">
-        <f>ROUND(SUM(C40:E40)-SUM(C49:E49),)</f>
-        <v>0</v>
-      </c>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="18"/>
-      <c r="G51" s="18"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="18" t="s">
+      <c r="B53" s="19">
+        <f>ROUND(SUM(C42:E42)-SUM(C51:E51),)</f>
+        <v>0</v>
+      </c>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B52" s="20"/>
-      <c r="C52" s="20">
-        <f>IF($B$51&gt;0,IF(LARGE($C$50:$F$50,$B$51)&lt;=C$50,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D52" s="20">
-        <f>IF(($B$51-C50)&gt;0,IF(LARGE($C$50:$F$50,$B$45)&lt;=D$50,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E52" s="20">
-        <f>IF(($B$51-SUM($C$50:$D$50))&gt;0,IF(LARGE($C$50:$F$50,$B$45)&lt;=E$50,1,0), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F52" s="18"/>
-      <c r="G52" s="18"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="19" t="s">
+      <c r="B54" s="19"/>
+      <c r="C54" s="19">
+        <f>IF($B$53&gt;0,IF(LARGE($C$52:$F$52,$B$53)&lt;=C$52,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D54" s="19">
+        <f>IF(($B$53-C52)&gt;0,IF(LARGE($C$52:$F$52,$B$47)&lt;=D$52,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E54" s="19">
+        <f>IF(($B$53-SUM($C$52:$D$52))&gt;0,IF(LARGE($C$52:$F$52,$B$47)&lt;=E$52,1,0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="17"/>
+      <c r="G54" s="17"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B53" s="19"/>
-      <c r="C53" s="19">
-        <f>C49+C52</f>
-        <v>0</v>
-      </c>
-      <c r="D53" s="19">
-        <f t="shared" ref="D53" si="8">D49+D52</f>
-        <v>236</v>
-      </c>
-      <c r="E53" s="19">
-        <f t="shared" ref="E53" si="9">E49+E52</f>
-        <v>0</v>
-      </c>
-      <c r="F53" s="19"/>
-      <c r="G53" s="19">
-        <f>SUM(C53:E53)</f>
-        <v>236</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="19" t="s">
+      <c r="B55" s="18"/>
+      <c r="C55" s="18">
+        <f>C51+C54</f>
+        <v>0</v>
+      </c>
+      <c r="D55" s="18">
+        <f t="shared" ref="D55" si="7">D51+D54</f>
+        <v>13</v>
+      </c>
+      <c r="E55" s="18">
+        <f t="shared" ref="E55" si="8">E51+E54</f>
+        <v>0</v>
+      </c>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18">
+        <f>SUM(C55:E55)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B55" s="19">
-        <f>G47+G53</f>
-        <v>1067</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B56" s="4"/>
+      <c r="B57" s="18">
+        <f>G49+G55</f>
+        <v>571</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B58" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A20:E21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feilende tester på fordeling av utbetaling
</commit_message>
<xml_diff>
--- a/doc/okonomi/Utbetaling-nyteknking.xlsx
+++ b/doc/okonomi/Utbetaling-nyteknking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/dev/nav/helse-spleis/doc/okonomi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2291667-85F1-FF49-BD5D-0566E5287648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DB5FFA-0374-A448-9FE3-F84D2C158B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="8400" windowWidth="58300" windowHeight="33100" xr2:uid="{D68530E5-53F4-9147-B78C-2EE89FEB1D81}"/>
+    <workbookView xWindow="12440" yWindow="7140" windowWidth="43220" windowHeight="33780" xr2:uid="{D68530E5-53F4-9147-B78C-2EE89FEB1D81}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -201,7 +201,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;NOK&quot;\ * #,##0.00_-;\-&quot;NOK&quot;\ * #,##0.00_-;_-&quot;NOK&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0000%"/>
-    <numFmt numFmtId="170" formatCode="0.000%"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -330,16 +330,16 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -658,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FF1C860-80D7-1E4E-BCDB-1C6933AA76C9}">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -707,14 +707,12 @@
         <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>30000</v>
+        <v>31000</v>
       </c>
       <c r="D5" s="1">
-        <v>10000</v>
-      </c>
-      <c r="E5" s="1">
-        <v>15000</v>
-      </c>
+        <v>31000</v>
+      </c>
+      <c r="E5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
@@ -724,15 +722,15 @@
       </c>
       <c r="C6" s="4">
         <f>C5*C7</f>
-        <v>30000</v>
+        <v>31000</v>
       </c>
       <c r="D6" s="4">
         <f>D5*D7</f>
-        <v>10000</v>
+        <v>31000</v>
       </c>
       <c r="E6" s="4">
         <f>E5*E7</f>
-        <v>15000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -761,15 +759,15 @@
       </c>
       <c r="C9" s="3">
         <f>C6/SUM($C$6:$E$6)</f>
-        <v>0.54545454545454541</v>
+        <v>0.5</v>
       </c>
       <c r="D9" s="3">
         <f>D6/SUM($C$6:$E$6)</f>
-        <v>0.18181818181818182</v>
+        <v>0.5</v>
       </c>
       <c r="E9" s="3">
         <f>E6/SUM($C$6:$E$6)</f>
-        <v>0.27272727272727271</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -779,15 +777,15 @@
       <c r="B10" s="9"/>
       <c r="C10" s="8">
         <f>$B$8*C9/12</f>
-        <v>25536.545454545452</v>
+        <v>23408.5</v>
       </c>
       <c r="D10" s="8">
         <f>$B$8*D9/12</f>
-        <v>8512.181818181818</v>
+        <v>23408.5</v>
       </c>
       <c r="E10" s="8">
         <f>$B$8*E9/12</f>
-        <v>12768.272727272726</v>
+        <v>0</v>
       </c>
       <c r="F10" t="s">
         <v>17</v>
@@ -799,15 +797,15 @@
       </c>
       <c r="C11" s="3">
         <f>C10/SUM($C$10:$E$10)</f>
-        <v>0.54545454545454541</v>
+        <v>0.5</v>
       </c>
       <c r="D11" s="3">
         <f>D10/SUM($C$10:$E$10)</f>
-        <v>0.18181818181818182</v>
+        <v>0.5</v>
       </c>
       <c r="E11" s="3">
         <f>E10/SUM($C$10:$E$10)</f>
-        <v>0.27272727272727271</v>
+        <v>0</v>
       </c>
       <c r="F11" t="s">
         <v>20</v>
@@ -828,21 +826,19 @@
         <v>29</v>
       </c>
       <c r="C13" s="11">
-        <f>30000*0.75</f>
-        <v>22500</v>
+        <v>15000</v>
       </c>
       <c r="D13" s="11">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="E13" s="11">
-        <f>E5</f>
-        <v>15000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="4">
         <f>12*SUM(C13:E13)</f>
-        <v>570000</v>
+        <v>180000</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -850,7 +846,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="4"/>
-      <c r="C15" s="26"/>
+      <c r="C15" s="24"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -858,15 +854,15 @@
       </c>
       <c r="C16" s="1">
         <f>MIN(C5,C13)</f>
-        <v>22500</v>
+        <v>15000</v>
       </c>
       <c r="D16" s="1">
         <f>MIN(D5,D13)</f>
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="E16" s="1">
         <f>MIN(E5,E13)</f>
-        <v>15000</v>
+        <v>0</v>
       </c>
       <c r="F16" t="s">
         <v>31</v>
@@ -879,15 +875,15 @@
       <c r="B17" s="9"/>
       <c r="C17" s="12">
         <f>IF(C5&gt;0,C16/C5,0)</f>
-        <v>0.75</v>
+        <v>0.4838709677419355</v>
       </c>
       <c r="D17" s="12">
         <f t="shared" ref="D17:E17" si="0">IF(D5&gt;0,D16/D5,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" s="12">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" t="s">
         <v>38</v>
@@ -899,44 +895,44 @@
       </c>
       <c r="C18" s="3">
         <f>C16/SUM($C$16:$E$16)</f>
-        <v>0.47368421052631576</v>
+        <v>1</v>
       </c>
       <c r="D18" s="3">
         <f>D16/SUM($C$16:$E$16)</f>
-        <v>0.21052631578947367</v>
+        <v>0</v>
       </c>
       <c r="E18" s="3">
         <f>E16/SUM($C$16:$E$16)</f>
-        <v>0.31578947368421051</v>
+        <v>0</v>
       </c>
       <c r="F18" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
     </row>
     <row r="20" spans="1:8" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -944,7 +940,7 @@
       </c>
       <c r="B22" s="1">
         <f>SUMPRODUCT($C$10:$E$10,$C$17:$E$17)</f>
-        <v>40432.863636363632</v>
+        <v>11326.693548387097</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -953,7 +949,7 @@
       </c>
       <c r="B23" s="1">
         <f>SUMPRODUCT($C$10:$E$10,$C$25:$E$25)</f>
-        <v>6384.1363636363631</v>
+        <v>35490.306451612902</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -961,16 +957,16 @@
         <v>7</v>
       </c>
       <c r="C24" s="13">
-        <f>C10*C17/$B$22</f>
-        <v>0.47368421052631576</v>
+        <f>12*C16/$B$14</f>
+        <v>1</v>
       </c>
       <c r="D24" s="13">
-        <f>D10*D17/$B$22</f>
-        <v>0.2105263157894737</v>
+        <f t="shared" ref="D24:E24" si="1">12*D16/$B$14</f>
+        <v>0</v>
       </c>
       <c r="E24" s="13">
-        <f>E10*E17/$B$22</f>
-        <v>0.31578947368421051</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="F24" t="s">
         <v>26</v>
@@ -983,15 +979,15 @@
       <c r="B25" s="4"/>
       <c r="C25" s="14">
         <f>(1-C17)</f>
-        <v>0.25</v>
+        <v>0.5161290322580645</v>
       </c>
       <c r="D25" s="14">
         <f>(1-D17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="14">
         <f>(1-E17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" t="s">
         <v>26</v>
@@ -1003,14 +999,14 @@
       </c>
       <c r="C26" s="13">
         <f>IF(SUMPRODUCT($C$10:$E$10,$C$25:$E$25)&gt;0,(C10*C25)/$B$23,0)</f>
-        <v>1</v>
+        <v>0.34042553191489366</v>
       </c>
       <c r="D26" s="13">
-        <f t="shared" ref="D26:E26" si="1">IF(SUMPRODUCT($C$10:$E$10,$C$25:$E$25)&gt;0,(D10*D25)/$B$23,0)</f>
-        <v>0</v>
+        <f t="shared" ref="D26:E26" si="2">IF(SUMPRODUCT($C$10:$E$10,$C$25:$E$25)&gt;0,(D10*D25)/$B$23,0)</f>
+        <v>0.65957446808510645</v>
       </c>
       <c r="E26" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1019,14 +1015,15 @@
         <v>8</v>
       </c>
       <c r="C28" s="2">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="D28" s="2">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E28" s="2">
-        <v>0.7</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F28" s="2"/>
       <c r="G28" s="10"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1035,16 +1032,17 @@
       </c>
       <c r="C29" s="6">
         <f>C28*C11</f>
-        <v>0.21818181818181817</v>
+        <v>0.4</v>
       </c>
       <c r="D29" s="6">
-        <f>D28*D11</f>
-        <v>9.0909090909090912E-2</v>
+        <f t="shared" ref="D29" si="3">D28*D11</f>
+        <v>0.3</v>
       </c>
       <c r="E29" s="6">
-        <f>E28*E11</f>
-        <v>0.19090909090909089</v>
-      </c>
+        <f t="shared" ref="E29" si="4">E28*E11</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="6"/>
       <c r="G29" s="4"/>
       <c r="H29" s="6"/>
     </row>
@@ -1058,15 +1056,15 @@
       <c r="B31" s="9"/>
       <c r="C31" s="15">
         <f>C24*C28 / SUMPRODUCT($C$24:$E$24,$C$28:$E$28)</f>
-        <v>0.36734693877551017</v>
+        <v>1</v>
       </c>
       <c r="D31" s="15">
         <f>D24*D28 / SUMPRODUCT($C$24:$E$24,$C$28:$E$28)</f>
-        <v>0.20408163265306123</v>
+        <v>0</v>
       </c>
       <c r="E31" s="15">
         <f>E24*E28 / SUMPRODUCT($C$24:$E$24,$C$28:$E$28)</f>
-        <v>0.42857142857142844</v>
+        <v>0</v>
       </c>
       <c r="F31" t="s">
         <v>18</v>
@@ -1078,15 +1076,15 @@
       </c>
       <c r="C32" s="3">
         <f>C11*C13*C28/SUMPRODUCT($C13:$E$13,$C$28:$E$28,$C$11:$E$11)</f>
-        <v>0.5654450261780104</v>
+        <v>1</v>
       </c>
       <c r="D32" s="3">
         <f>D11*D13*D28/SUMPRODUCT($C13:$E$13,$C$28:$E$28,$C$11:$E$11)</f>
-        <v>0.10471204188481675</v>
+        <v>0</v>
       </c>
       <c r="E32" s="3">
         <f>E11*E13*E28/SUMPRODUCT($C13:$E$13,$C$28:$E$28,$C$11:$E$11)</f>
-        <v>0.32984293193717268</v>
+        <v>0</v>
       </c>
       <c r="F32" t="s">
         <v>24</v>
@@ -1099,11 +1097,11 @@
       <c r="B33" s="9"/>
       <c r="C33" s="12">
         <f>IF(SUMPRODUCT($C$26:$E$26,$C$28:$E$28)&gt;0,(C26*C28) / SUMPRODUCT($C$26:$E$26,$C$28:$E$28),0)</f>
-        <v>1</v>
+        <v>0.40764331210191085</v>
       </c>
       <c r="D33" s="12">
         <f>IF(SUMPRODUCT($C$26:$E$26,$C$28:$E$28)&gt;0,(D26*D28) / SUMPRODUCT($C$26:$E$26,$C$28:$E$28),0)</f>
-        <v>0</v>
+        <v>0.59235668789808915</v>
       </c>
       <c r="E33" s="12">
         <f>IF(SUMPRODUCT($C$26:$E$26,$C$28:$E$28)&gt;0,(E26*E28) / SUMPRODUCT($C$26:$E$26,$C$28:$E$28),0)</f>
@@ -1116,7 +1114,7 @@
       </c>
       <c r="B34" s="16">
         <f>SUM(C29:E29)</f>
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="E34" s="4"/>
     </row>
@@ -1126,7 +1124,7 @@
       </c>
       <c r="B35" s="6">
         <f>MIN(1,B36/B37)</f>
-        <v>1</v>
+        <v>0.36616735679042106</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -1138,11 +1136,11 @@
       </c>
       <c r="B36" s="1">
         <f>12*SUMPRODUCT(C6:E6,C28:E28,C17:E17)</f>
-        <v>294000</v>
+        <v>144000</v>
       </c>
       <c r="C36" s="1">
         <f>SUMPRODUCT(C16:E16,C28:E28)*12</f>
-        <v>294000</v>
+        <v>144000</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>51</v>
@@ -1154,11 +1152,11 @@
       </c>
       <c r="B37" s="4">
         <f>B12*B34</f>
-        <v>280902</v>
+        <v>393262.8</v>
       </c>
       <c r="C37" s="4">
         <f>B37/260</f>
-        <v>1080.3923076923077</v>
+        <v>1512.5492307692307</v>
       </c>
       <c r="D37" s="4"/>
     </row>
@@ -1168,11 +1166,11 @@
       </c>
       <c r="B38" s="4">
         <f>ROUND(B37/260,)*260</f>
-        <v>280800</v>
+        <v>393380</v>
       </c>
       <c r="C38" s="4">
         <f>B38/260</f>
-        <v>1080</v>
+        <v>1513</v>
       </c>
       <c r="F38" t="s">
         <v>39</v>
@@ -1184,7 +1182,7 @@
       </c>
       <c r="B39" s="4">
         <f>B38*B35</f>
-        <v>280800</v>
+        <v>144042.91481421582</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -1193,7 +1191,7 @@
       </c>
       <c r="B40" s="4">
         <f>B38-B39</f>
-        <v>0</v>
+        <v>249337.08518578418</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
@@ -1206,20 +1204,20 @@
       <c r="B41" s="17"/>
       <c r="C41" s="20">
         <f>$B$39*C31/260</f>
-        <v>396.73469387755097</v>
+        <v>554.01121082390705</v>
       </c>
       <c r="D41" s="20">
         <f>$B$39*D31/260</f>
-        <v>220.40816326530611</v>
+        <v>0</v>
       </c>
       <c r="E41" s="20">
         <f>$B$39*E31/260</f>
-        <v>462.85714285714272</v>
+        <v>0</v>
       </c>
       <c r="F41" s="17"/>
       <c r="G41" s="17">
         <f>SUM(C41:E41)</f>
-        <v>1079.9999999999998</v>
+        <v>554.01121082390705</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -1229,11 +1227,11 @@
       <c r="B42" s="17"/>
       <c r="C42" s="20">
         <f>$B$40*C33/260</f>
-        <v>0</v>
+        <v>390.9253662883437</v>
       </c>
       <c r="D42" s="20">
         <f>$B$40*D33/260</f>
-        <v>0</v>
+        <v>568.06342288774943</v>
       </c>
       <c r="E42" s="20">
         <f>$B$40*E33/260</f>
@@ -1242,7 +1240,7 @@
       <c r="F42" s="17"/>
       <c r="G42" s="17">
         <f>SUM(C42:E42)</f>
-        <v>0</v>
+        <v>958.98878917609318</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -1252,20 +1250,20 @@
       </c>
       <c r="C43" s="19">
         <f>SUM(C41:C42)</f>
-        <v>396.73469387755097</v>
+        <v>944.93657711225069</v>
       </c>
       <c r="D43" s="19">
-        <f t="shared" ref="D43:E43" si="2">SUM(D41:D42)</f>
-        <v>220.40816326530611</v>
+        <f t="shared" ref="D43:E43" si="5">SUM(D41:D42)</f>
+        <v>568.06342288774943</v>
       </c>
       <c r="E43" s="19">
-        <f t="shared" si="2"/>
-        <v>462.85714285714272</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="F43" s="17"/>
       <c r="G43" s="17">
         <f>SUM(G41:G42)</f>
-        <v>1079.9999999999998</v>
+        <v>1513.0000000000002</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -1284,43 +1282,43 @@
       <c r="B45" s="17"/>
       <c r="C45" s="20">
         <f>TRUNC(C41)</f>
-        <v>396</v>
+        <v>554</v>
       </c>
       <c r="D45" s="19">
-        <f t="shared" ref="D45:E45" si="3">TRUNC(D41)</f>
-        <v>220</v>
+        <f t="shared" ref="D45:E45" si="6">TRUNC(D41)</f>
+        <v>0</v>
       </c>
       <c r="E45" s="19">
-        <f t="shared" si="3"/>
-        <v>462</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="F45" s="17"/>
-      <c r="G45" s="24">
+      <c r="G45" s="22">
         <f>SUM(C45:E45)</f>
-        <v>1078</v>
+        <v>554</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B46" s="24"/>
+      <c r="B46" s="22"/>
       <c r="C46" s="19">
         <f>C41-C45</f>
-        <v>0.73469387755096704</v>
+        <v>1.1210823907049416E-2</v>
       </c>
       <c r="D46" s="19">
-        <f t="shared" ref="D46:E46" si="4">D41-D45</f>
-        <v>0.40816326530611491</v>
+        <f t="shared" ref="D46:E46" si="7">D41-D45</f>
+        <v>0</v>
       </c>
       <c r="E46" s="19">
-        <f t="shared" si="4"/>
-        <v>0.85714285714271909</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
       <c r="F46" s="17"/>
       <c r="G46" s="17">
         <f>SUM(C46:E46)</f>
-        <v>1.999999999999801</v>
+        <v>1.1210823907049416E-2</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -1329,7 +1327,7 @@
       </c>
       <c r="B47" s="20">
         <f>ROUND(SUM(C41:E41)-SUM(C45:E45),)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C47" s="19"/>
       <c r="D47" s="19"/>
@@ -1344,7 +1342,7 @@
       <c r="B48" s="17"/>
       <c r="C48" s="19">
         <f>IF($B$47&gt;0,IF(LARGE($C$46:$F$46,$B$47)&lt;=C$46,1,0), 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48" s="19">
         <f>IF(($B$47-C48)&gt;0,IF(LARGE($C$46:$F$46,$B$47)&lt;=D$46,1,0), 0)</f>
@@ -1352,7 +1350,7 @@
       </c>
       <c r="E48" s="19">
         <f>IF(($B$47-SUM($C$48:$D$48))&gt;0,IF(LARGE($C$46:$F$46,$B$47)&lt;=E$46,1,0), 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F48" s="17"/>
       <c r="G48" s="17"/>
@@ -1362,22 +1360,22 @@
         <v>43</v>
       </c>
       <c r="B49" s="18"/>
-      <c r="C49" s="25">
+      <c r="C49" s="23">
         <f>C45+C48</f>
-        <v>397</v>
+        <v>554</v>
       </c>
       <c r="D49" s="18">
-        <f t="shared" ref="D49:E49" si="5">D45+D48</f>
-        <v>220</v>
+        <f t="shared" ref="D49:E49" si="8">D45+D48</f>
+        <v>0</v>
       </c>
       <c r="E49" s="18">
-        <f t="shared" si="5"/>
-        <v>463</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="F49" s="18"/>
       <c r="G49" s="18">
         <f>SUM(C49:E49)</f>
-        <v>1080</v>
+        <v>554</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -1396,20 +1394,20 @@
       <c r="B51" s="19"/>
       <c r="C51" s="20">
         <f>TRUNC(C42)</f>
-        <v>0</v>
+        <v>390</v>
       </c>
       <c r="D51" s="19">
-        <f t="shared" ref="D51:E51" si="6">TRUNC(D42)</f>
-        <v>0</v>
+        <f t="shared" ref="D51:E51" si="9">TRUNC(D42)</f>
+        <v>568</v>
       </c>
       <c r="E51" s="19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F51" s="17"/>
-      <c r="G51" s="24">
+      <c r="G51" s="22">
         <f>SUM(C51:E51)</f>
-        <v>0</v>
+        <v>958</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
@@ -1419,29 +1417,29 @@
       <c r="B52" s="19"/>
       <c r="C52" s="19">
         <f>C42-C51</f>
-        <v>0</v>
+        <v>0.92536628834369594</v>
       </c>
       <c r="D52" s="19">
-        <f t="shared" ref="D52:E52" si="7">D42-D51</f>
-        <v>0</v>
+        <f t="shared" ref="D52:E52" si="10">D42-D51</f>
+        <v>6.3422887749425172E-2</v>
       </c>
       <c r="E52" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F52" s="17"/>
       <c r="G52" s="17">
         <f>SUM(C52:E52)</f>
-        <v>0</v>
+        <v>0.98878917609312111</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B53" s="23">
+      <c r="B53" s="21">
         <f>C38-G49-G51</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C53" s="19"/>
       <c r="D53" s="19"/>
@@ -1456,14 +1454,14 @@
       <c r="B54" s="19"/>
       <c r="C54" s="19">
         <f>IF($B$53&gt;0,IF(LARGE($C$52:$F$52,$B$53)&lt;=C$52,1,0), 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D54" s="19">
-        <f>IF(($B$53-C52)&gt;0,IF(LARGE($C$52:$F$52,$B$47)&lt;=D$52,1,0), 0)</f>
+        <f>IF(($B$53-C54)&gt;0,IF(LARGE($C$52:$F$52,$B$47)&lt;=D$52,1,0), 0)</f>
         <v>0</v>
       </c>
       <c r="E54" s="19">
-        <f>IF(($B$53-SUM($C$52:$D$52))&gt;0,IF(LARGE($C$52:$F$52,$B$47)&lt;=E$52,1,0), 0)</f>
+        <f>IF(($B$53-SUM($C$54:$D$54))&gt;0,IF(LARGE($C$52:$F$52,$B$47)&lt;=E$52,1,0), 0)</f>
         <v>0</v>
       </c>
       <c r="F54" s="17"/>
@@ -1476,20 +1474,20 @@
       <c r="B55" s="18"/>
       <c r="C55" s="18">
         <f>C51+C54</f>
-        <v>0</v>
+        <v>391</v>
       </c>
       <c r="D55" s="18">
-        <f t="shared" ref="D55" si="8">D51+D54</f>
-        <v>0</v>
+        <f t="shared" ref="D55" si="11">D51+D54</f>
+        <v>568</v>
       </c>
       <c r="E55" s="18">
-        <f t="shared" ref="E55" si="9">E51+E54</f>
+        <f t="shared" ref="E55" si="12">E51+E54</f>
         <v>0</v>
       </c>
       <c r="F55" s="18"/>
       <c r="G55" s="18">
         <f>SUM(C55:E55)</f>
-        <v>0</v>
+        <v>959</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -1498,7 +1496,7 @@
       </c>
       <c r="B57" s="18">
         <f>G49+G55</f>
-        <v>1080</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>